<commit_message>
Deploying to gh-pages from  @ 0cbbda99f8f91f719286dc764217299536694454 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/10.2.1.xlsx
+++ b/en/downloads/data-excel/10.2.1.xlsx
@@ -757,9 +757,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
   <cols>
@@ -767,7 +769,7 @@
     <col min="4" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="51" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="51" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>26</v>
       </c>
@@ -778,7 +780,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -789,7 +791,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -799,8 +801,9 @@
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
-    </row>
-    <row r="4" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
@@ -828,8 +831,11 @@
       <c r="I4" s="9">
         <v>2020</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="J4" s="9">
+        <v>2021</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>30</v>
       </c>
@@ -857,8 +863,11 @@
       <c r="I5" s="26">
         <v>4700.5</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" s="5" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="J5" s="6">
+        <v>5356.3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="5" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>29</v>
       </c>
@@ -886,8 +895,11 @@
       <c r="I6" s="27">
         <v>10.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="J6" s="5">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>33</v>
       </c>
@@ -904,7 +916,7 @@
       <c r="H7" s="19"/>
       <c r="I7" s="27"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>35</v>
       </c>
@@ -932,8 +944,11 @@
       <c r="I8" s="28">
         <v>8.4</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="2">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>36</v>
       </c>
@@ -961,8 +976,11 @@
       <c r="I9" s="28">
         <v>11.6</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="2">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
         <v>72</v>
       </c>
@@ -979,7 +997,7 @@
       <c r="H10" s="14"/>
       <c r="I10" s="28"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>37</v>
       </c>
@@ -1007,8 +1025,11 @@
       <c r="I11" s="28">
         <v>10.6</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" s="2">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>38</v>
       </c>
@@ -1036,8 +1057,11 @@
       <c r="I12" s="28">
         <v>10.3</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" s="2">
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
         <v>73</v>
       </c>
@@ -1054,7 +1078,7 @@
       <c r="H13" s="14"/>
       <c r="I13" s="28"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>61</v>
       </c>
@@ -1082,8 +1106,11 @@
       <c r="I14" s="28">
         <v>16.3</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" s="2">
+        <v>14.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>62</v>
       </c>
@@ -1111,8 +1138,11 @@
       <c r="I15" s="28">
         <v>10.8</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J15" s="2">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>67</v>
       </c>
@@ -1140,8 +1170,11 @@
       <c r="I16" s="28">
         <v>10.7</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J16" s="2">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>68</v>
       </c>
@@ -1169,8 +1202,11 @@
       <c r="I17" s="28">
         <v>8.1999999999999993</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J17" s="2">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>74</v>
       </c>
@@ -1187,7 +1223,7 @@
       <c r="H18" s="14"/>
       <c r="I18" s="28"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>43</v>
       </c>
@@ -1216,7 +1252,7 @@
         <v>11.755326439375899</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>44</v>
       </c>
@@ -1245,7 +1281,7 @@
         <v>18.008531163794252</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>45</v>
       </c>
@@ -1274,7 +1310,7 @@
         <v>12.860319584844115</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>46</v>
       </c>
@@ -1303,7 +1339,7 @@
         <v>27.855975107092345</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>47</v>
       </c>
@@ -1332,7 +1368,7 @@
         <v>3.8567050275050248</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>48</v>
       </c>
@@ -1361,7 +1397,7 @@
         <v>12.700277251528242</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>49</v>
       </c>
@@ -1390,7 +1426,7 @@
         <v>6.543625743604494</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>50</v>
       </c>
@@ -1419,7 +1455,7 @@
         <v>7.921875108777849</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
         <v>51</v>
       </c>
@@ -1447,6 +1483,7 @@
       <c r="I27" s="30">
         <v>6.2551885850595959</v>
       </c>
+      <c r="J27" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ 41789f4f1f146d5e6b766d4572a23765b0275b21 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/10.2.1.xlsx
+++ b/en/downloads/data-excel/10.2.1.xlsx
@@ -760,7 +760,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L27" sqref="L27"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -1251,6 +1251,9 @@
       <c r="I19" s="29">
         <v>11.755326439375899</v>
       </c>
+      <c r="J19" s="28">
+        <v>12.434613462352335</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
@@ -1280,6 +1283,9 @@
       <c r="I20" s="29">
         <v>18.008531163794252</v>
       </c>
+      <c r="J20" s="28">
+        <v>16.80050595536094</v>
+      </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
@@ -1309,6 +1315,9 @@
       <c r="I21" s="29">
         <v>12.860319584844115</v>
       </c>
+      <c r="J21" s="28">
+        <v>11.282963378125267</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
@@ -1338,6 +1347,9 @@
       <c r="I22" s="29">
         <v>27.855975107092345</v>
       </c>
+      <c r="J22" s="28">
+        <v>25.042808754677555</v>
+      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
@@ -1367,6 +1379,9 @@
       <c r="I23" s="29">
         <v>3.8567050275050248</v>
       </c>
+      <c r="J23" s="28">
+        <v>3.2011163356916352</v>
+      </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
@@ -1396,6 +1411,9 @@
       <c r="I24" s="29">
         <v>12.700277251528242</v>
       </c>
+      <c r="J24" s="28">
+        <v>13.523574517571838</v>
+      </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
@@ -1425,6 +1443,9 @@
       <c r="I25" s="29">
         <v>6.543625743604494</v>
       </c>
+      <c r="J25" s="28">
+        <v>6.1196997869329204</v>
+      </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
@@ -1454,6 +1475,9 @@
       <c r="I26" s="29">
         <v>7.921875108777849</v>
       </c>
+      <c r="J26" s="28">
+        <v>5.9488136666578013</v>
+      </c>
     </row>
     <row r="27" spans="1:10" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
@@ -1483,7 +1507,9 @@
       <c r="I27" s="30">
         <v>6.2551885850595959</v>
       </c>
-      <c r="J27" s="30"/>
+      <c r="J27" s="30">
+        <v>5.2451982064110645</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Deploying to gh-pages from  @ eebb8279b094d222a9f07d22016969811150b3ce 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/10.2.1.xlsx
+++ b/en/downloads/data-excel/10.2.1.xlsx
@@ -354,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
@@ -445,6 +445,21 @@
     </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -757,10 +772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -769,7 +784,7 @@
     <col min="4" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="51" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="51" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>26</v>
       </c>
@@ -780,7 +795,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -791,7 +806,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -802,8 +817,9 @@
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
-    </row>
-    <row r="4" spans="1:10" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K3" s="4"/>
+    </row>
+    <row r="4" spans="1:11" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
@@ -834,8 +850,11 @@
       <c r="J4" s="9">
         <v>2021</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="K4" s="31">
+        <v>2022</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="6" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>30</v>
       </c>
@@ -866,8 +885,11 @@
       <c r="J5" s="6">
         <v>5356.3</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" s="5" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="K5" s="32">
+        <v>6512.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="5" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
         <v>29</v>
       </c>
@@ -898,8 +920,11 @@
       <c r="J6" s="5">
         <v>9.5</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K6" s="33">
+        <v>9.2524142373849365</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
         <v>33</v>
       </c>
@@ -916,7 +941,7 @@
       <c r="H7" s="19"/>
       <c r="I7" s="27"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>35</v>
       </c>
@@ -947,8 +972,11 @@
       <c r="J8" s="2">
         <v>7.9</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K8" s="32">
+        <v>9.1726448995762642</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>36</v>
       </c>
@@ -979,8 +1007,11 @@
       <c r="J9" s="2">
         <v>10.5</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K9" s="32">
+        <v>9.2988242598562199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="23" t="s">
         <v>72</v>
       </c>
@@ -997,7 +1028,7 @@
       <c r="H10" s="14"/>
       <c r="I10" s="28"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>37</v>
       </c>
@@ -1028,8 +1059,11 @@
       <c r="J11" s="2">
         <v>9.6</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K11" s="32">
+        <v>9.3929513987987647</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>38</v>
       </c>
@@ -1060,8 +1094,11 @@
       <c r="J12" s="2">
         <v>9.4</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K12" s="32">
+        <v>9.0963110935638873</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="23" t="s">
         <v>73</v>
       </c>
@@ -1078,7 +1115,7 @@
       <c r="H13" s="14"/>
       <c r="I13" s="28"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>61</v>
       </c>
@@ -1109,8 +1146,11 @@
       <c r="J14" s="2">
         <v>14.8</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K14" s="32">
+        <v>12.819848845068858</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
         <v>62</v>
       </c>
@@ -1141,8 +1181,11 @@
       <c r="J15" s="2">
         <v>9.1</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K15" s="32">
+        <v>7.8843953890120773</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="21" t="s">
         <v>67</v>
       </c>
@@ -1173,8 +1216,11 @@
       <c r="J16" s="2">
         <v>9.5</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K16" s="28">
+        <v>7.6890997954400655</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="21" t="s">
         <v>68</v>
       </c>
@@ -1205,8 +1251,11 @@
       <c r="J17" s="2">
         <v>5.9</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K17" s="32">
+        <v>4.859109337853182</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
         <v>74</v>
       </c>
@@ -1223,7 +1272,7 @@
       <c r="H18" s="14"/>
       <c r="I18" s="28"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>43</v>
       </c>
@@ -1254,8 +1303,11 @@
       <c r="J19" s="28">
         <v>12.434613462352335</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K19" s="34">
+        <v>12.268952512062626</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>44</v>
       </c>
@@ -1286,8 +1338,11 @@
       <c r="J20" s="28">
         <v>16.80050595536094</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K20" s="34">
+        <v>8.8432516850244731</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>45</v>
       </c>
@@ -1318,8 +1373,11 @@
       <c r="J21" s="28">
         <v>11.282963378125267</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K21" s="34">
+        <v>12.356872582336921</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>46</v>
       </c>
@@ -1350,8 +1408,11 @@
       <c r="J22" s="28">
         <v>25.042808754677555</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K22" s="34">
+        <v>25.295368484771757</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>47</v>
       </c>
@@ -1382,8 +1443,11 @@
       <c r="J23" s="28">
         <v>3.2011163356916352</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K23" s="34">
+        <v>4.2612456375718351</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>48</v>
       </c>
@@ -1414,8 +1478,11 @@
       <c r="J24" s="28">
         <v>13.523574517571838</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K24" s="34">
+        <v>14.933279226285201</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>49</v>
       </c>
@@ -1446,8 +1513,11 @@
       <c r="J25" s="28">
         <v>6.1196997869329204</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K25" s="34">
+        <v>9.0993456624506877</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>50</v>
       </c>
@@ -1478,8 +1548,11 @@
       <c r="J26" s="28">
         <v>5.9488136666578013</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K26" s="34">
+        <v>6.7003522302183303</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="12.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="12" t="s">
         <v>51</v>
       </c>
@@ -1509,6 +1582,9 @@
       </c>
       <c r="J27" s="30">
         <v>5.2451982064110645</v>
+      </c>
+      <c r="K27" s="35">
+        <v>12.078370902890091</v>
       </c>
     </row>
   </sheetData>

</xml_diff>